<commit_message>
updated templates and rda object
</commit_message>
<xml_diff>
--- a/ISRaD_Data/Basile_Doelsch_2005.xlsx
+++ b/ISRaD_Data/Basile_Doelsch_2005.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21060" windowHeight="14800" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21060" windowHeight="14800" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="954">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1384" uniqueCount="954">
   <si>
     <t>entry_name</t>
   </si>
@@ -3566,11 +3566,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ5"/>
+  <dimension ref="A1:AJ4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:36">
       <c r="A1" t="s">
@@ -3912,6 +3917,9 @@
       <c r="P4" t="s">
         <v>166</v>
       </c>
+      <c r="Q4" t="s">
+        <v>170</v>
+      </c>
       <c r="T4" t="s">
         <v>167</v>
       </c>
@@ -3919,44 +3927,6 @@
         <v>168</v>
       </c>
       <c r="AA4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="5" spans="1:36">
-      <c r="A5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" t="s">
-        <v>161</v>
-      </c>
-      <c r="H5" t="s">
-        <v>162</v>
-      </c>
-      <c r="L5" t="s">
-        <v>163</v>
-      </c>
-      <c r="M5" t="s">
-        <v>164</v>
-      </c>
-      <c r="N5" t="s">
-        <v>165</v>
-      </c>
-      <c r="P5" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>170</v>
-      </c>
-      <c r="T5" t="s">
-        <v>167</v>
-      </c>
-      <c r="U5" t="s">
-        <v>168</v>
-      </c>
-      <c r="AA5" t="s">
         <v>169</v>
       </c>
     </row>
@@ -5874,7 +5844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+    <sheetView topLeftCell="AC1" workbookViewId="0">
       <selection activeCell="AI1" sqref="AI1:AK1"/>
     </sheetView>
   </sheetViews>

</xml_diff>